<commit_message>
removing grades file from git
</commit_message>
<xml_diff>
--- a/Participation-Tracker.xlsx
+++ b/Participation-Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joser\OneDrive\Documents\EC-311\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92461D5B-CFAE-4471-9D04-0B357405E5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75863789-FA6A-4388-B792-DAB1A22E3D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="92">
   <si>
     <t>Student</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>Exams</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -1196,25 +1199,25 @@
   <dimension ref="A1:AT48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="7.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7265625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1287,9 +1290,11 @@
       <c r="D2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F2" s="1">
-        <f>ROUND(COUNTIF(C2:E2, "Y")/COUNTA($C$1:$E$1)*5,2)</f>
+        <f>ROUND(COUNTIF(C2:E2, "Y")/COUNTA(C2:E2)*5,2)</f>
         <v>0</v>
       </c>
       <c r="G2" s="2">
@@ -1324,17 +1329,19 @@
       <c r="D3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F46" si="0">ROUND(COUNTIF(C3:E3, "Y")/COUNTA($C$1:$E$1)*5,2)</f>
-        <v>1.67</v>
+        <f>ROUND(COUNTIF(C3:E3, "Y")/COUNTA(C3:E3)*5,2)</f>
+        <v>3.33</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G46" si="1">F3+H3</f>
-        <v>2.17</v>
+        <f t="shared" ref="G3:G46" si="0">F3+H3</f>
+        <v>3.83</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H46" si="2">COUNTIF(I3:R3,"Y")*0.5</f>
+        <f t="shared" ref="H3:H46" si="1">COUNTIF(I3:R3,"Y")*0.5</f>
         <v>0.5</v>
       </c>
       <c r="I3" s="2"/>
@@ -1363,17 +1370,19 @@
       <c r="D4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f>ROUND(COUNTIF(C4:E4, "Y")/COUNTA(C4:E4)*5,2)</f>
+        <v>5</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" si="1"/>
-        <v>3.33</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I4" s="2"/>
@@ -1400,17 +1409,19 @@
       <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" ref="F5:F46" si="2">ROUND(COUNTIF(C5:E5, "Y")/COUNTA(C5:E5)*5,2)</f>
+        <v>5</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="1"/>
-        <v>4.33</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1441,17 +1452,19 @@
       <c r="D6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I6" s="2"/>
@@ -1478,18 +1491,20 @@
       <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="1"/>
-        <v>5.33</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
@@ -1505,8 +1520,12 @@
       <c r="N7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="4"/>
     </row>
@@ -1523,17 +1542,19 @@
       <c r="D8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="1"/>
-        <v>3.83</v>
+        <f t="shared" si="0"/>
+        <v>5.5</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="I8" s="2"/>
@@ -1562,17 +1583,19 @@
       <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="1"/>
-        <v>4.33</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -1607,15 +1630,15 @@
         <v>48</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I10" s="2"/>
@@ -1642,18 +1665,20 @@
       <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F11" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="1"/>
-        <v>5.33</v>
+        <f t="shared" si="0"/>
+        <v>7.5</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>2.5</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>48</v>
@@ -1669,7 +1694,9 @@
         <v>48</v>
       </c>
       <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="O11" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="4"/>
@@ -1687,18 +1714,20 @@
       <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F12" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="1"/>
-        <v>6.33</v>
+        <f t="shared" si="0"/>
+        <v>8.5</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>3.5</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>48</v>
@@ -1718,7 +1747,9 @@
       <c r="N12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O12" s="2"/>
+      <c r="O12" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="4"/>
@@ -1740,15 +1771,15 @@
         <v>49</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.67</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I13" s="2"/>
@@ -1775,17 +1806,19 @@
       <c r="D14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I14" s="2"/>
@@ -1816,16 +1849,16 @@
         <v>48</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>48</v>
@@ -1841,8 +1874,12 @@
       <c r="N15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
+      <c r="O15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="4"/>
       <c r="AI15" s="2" t="s">
@@ -1891,18 +1928,20 @@
       <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F16" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="1"/>
-        <v>4.83</v>
+        <f t="shared" si="0"/>
+        <v>7.5</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+        <f t="shared" si="1"/>
+        <v>2.5</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1916,22 +1955,26 @@
       <c r="N16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="O16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="4"/>
       <c r="AI16" s="1" t="s">
         <v>67</v>
       </c>
       <c r="AJ16" s="1">
-        <v>11.95</v>
+        <v>14.8</v>
       </c>
       <c r="AK16" s="1">
         <v>15</v>
       </c>
       <c r="AL16" s="3">
         <f>ROUND(AJ16/AK16,2)</f>
-        <v>0.8</v>
+        <v>0.99</v>
       </c>
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
@@ -1968,18 +2011,20 @@
       <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F17" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="1"/>
-        <v>3.33</v>
+        <f t="shared" si="0"/>
+        <v>5.5</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1988,14 +2033,16 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+      <c r="P17" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="4"/>
       <c r="AI17" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AJ17" s="1">
-        <v>12.95</v>
+        <v>12.85</v>
       </c>
       <c r="AK17" s="1">
         <v>15</v>
@@ -2008,26 +2055,26 @@
       <c r="AN17" s="1"/>
       <c r="AO17" s="1">
         <f>AL24*AO16</f>
-        <v>19.2</v>
+        <v>19</v>
       </c>
       <c r="AP17" s="1">
         <f>ROUND(AL34*AP16,2)</f>
-        <v>13.75</v>
+        <v>12.75</v>
       </c>
       <c r="AQ17" s="1">
         <f>AL37*AQ16</f>
-        <v>8.25</v>
+        <v>21.75</v>
       </c>
       <c r="AR17" s="1">
         <f>AL38*AR16</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AS17" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AT17" s="1">
         <f>SUM(AO17:AS17)</f>
-        <v>79.2</v>
+        <v>78.5</v>
       </c>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.35">
@@ -2043,17 +2090,19 @@
       <c r="D18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F18" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="1"/>
-        <v>3.33</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I18" s="2"/>
@@ -2070,14 +2119,14 @@
         <v>69</v>
       </c>
       <c r="AJ18" s="1">
-        <v>14.85</v>
+        <v>13.95</v>
       </c>
       <c r="AK18" s="1">
         <v>15</v>
       </c>
       <c r="AL18" s="3">
         <f t="shared" si="3"/>
-        <v>0.99</v>
+        <v>0.93</v>
       </c>
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
@@ -2105,16 +2154,16 @@
         <v>48</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2126,14 +2175,18 @@
       <c r="N19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
+      <c r="O19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="4"/>
       <c r="AI19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AJ19" s="5">
+      <c r="AJ19" s="1">
         <v>15</v>
       </c>
       <c r="AK19" s="1">
@@ -2169,15 +2222,15 @@
         <v>48</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I20" s="2"/>
@@ -2193,15 +2246,15 @@
       <c r="AI20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AJ20" s="5">
-        <v>15</v>
+      <c r="AJ20" s="1">
+        <v>12.58</v>
       </c>
       <c r="AK20" s="1">
         <v>15</v>
       </c>
       <c r="AL20" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
       <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
@@ -2225,17 +2278,19 @@
       <c r="D21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F21" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f>ROUND(COUNTIF(C21:E21, "Y")/COUNTA(C21:E21)*5,2)</f>
+        <v>5</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="1"/>
-        <v>3.33</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I21" s="2"/>
@@ -2252,14 +2307,14 @@
         <v>72</v>
       </c>
       <c r="AJ21" s="5">
-        <v>15</v>
+        <v>14.89</v>
       </c>
       <c r="AK21" s="1">
         <v>15</v>
       </c>
       <c r="AL21" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
@@ -2287,15 +2342,15 @@
         <v>48</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I22" s="2"/>
@@ -2312,7 +2367,7 @@
         <v>73</v>
       </c>
       <c r="AJ22" s="5">
-        <v>15</v>
+        <v>14.95</v>
       </c>
       <c r="AK22" s="1">
         <v>15</v>
@@ -2343,18 +2398,20 @@
       <c r="D23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F23" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="1"/>
-        <v>6.33</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>48</v>
@@ -2374,8 +2431,12 @@
       <c r="N23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
+      <c r="O23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="4"/>
       <c r="AI23" s="1" t="s">
@@ -2413,17 +2474,19 @@
       <c r="D24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="F24" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="1"/>
-        <v>3.33</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I24" s="2"/>
@@ -2439,7 +2502,7 @@
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1">
         <f>SUM(AJ16:AJ23)</f>
-        <v>114.75</v>
+        <v>114.02</v>
       </c>
       <c r="AK24" s="1">
         <f>SUM(AK16:AK23)</f>
@@ -2447,7 +2510,7 @@
       </c>
       <c r="AL24" s="3">
         <f t="shared" si="3"/>
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
@@ -2471,18 +2534,20 @@
       <c r="D25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F25" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="1"/>
-        <v>5.83</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="2"/>
-        <v>2.5</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>48</v>
@@ -2499,9 +2564,15 @@
       <c r="M25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
+      <c r="N25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="4"/>
       <c r="AI25" s="1"/>
@@ -2530,18 +2601,20 @@
       <c r="D26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F26" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="1"/>
-        <v>4.83</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>48</v>
@@ -2555,7 +2628,9 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
+      <c r="O26" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="4"/>
@@ -2597,16 +2672,16 @@
         <v>48</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>48</v>
@@ -2626,8 +2701,12 @@
       <c r="N27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
+      <c r="O27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="4"/>
       <c r="AI27" s="1" t="s">
@@ -2669,15 +2748,15 @@
         <v>48</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.33</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.33</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I28" s="2"/>
@@ -2694,14 +2773,14 @@
         <v>76</v>
       </c>
       <c r="AJ28" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AK28" s="1">
         <v>10</v>
       </c>
       <c r="AL28" s="3">
         <f t="shared" si="4"/>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="AM28" s="1"/>
       <c r="AN28" s="1"/>
@@ -2729,15 +2808,15 @@
         <v>48</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.67</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I29" s="2"/>
@@ -2753,9 +2832,16 @@
       <c r="AI29" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AJ29" s="1"/>
-      <c r="AK29" s="1"/>
-      <c r="AL29" s="3"/>
+      <c r="AJ29" s="1">
+        <v>7</v>
+      </c>
+      <c r="AK29" s="1">
+        <v>10</v>
+      </c>
+      <c r="AL29" s="3">
+        <f t="shared" si="4"/>
+        <v>0.7</v>
+      </c>
       <c r="AM29" s="1"/>
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
@@ -2778,18 +2864,20 @@
       <c r="D30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F30" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G30" s="2">
-        <f t="shared" si="1"/>
-        <v>4.83</v>
+        <f t="shared" si="0"/>
+        <v>7.5</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+        <f t="shared" si="1"/>
+        <v>2.5</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>48</v>
@@ -2803,22 +2891,26 @@
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
+      <c r="O30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="4"/>
       <c r="AI30" s="1" t="s">
         <v>78</v>
       </c>
       <c r="AJ30" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AK30" s="1">
         <v>10</v>
       </c>
       <c r="AL30" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AM30" s="1"/>
       <c r="AN30" s="1"/>
@@ -2842,18 +2934,20 @@
       <c r="D31" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="1"/>
-        <v>3.17</v>
+        <f t="shared" si="0"/>
+        <v>4.17</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+        <f t="shared" si="1"/>
+        <v>2.5</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2" t="s">
@@ -2867,23 +2961,20 @@
         <v>48</v>
       </c>
       <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
+      <c r="O31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="4"/>
       <c r="AI31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AJ31" s="5">
-        <v>10</v>
-      </c>
-      <c r="AK31" s="1">
-        <v>10</v>
-      </c>
-      <c r="AL31" s="3">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
+      <c r="AJ31" s="1"/>
+      <c r="AK31" s="1"/>
+      <c r="AL31" s="3"/>
       <c r="AM31" s="1"/>
       <c r="AN31" s="1"/>
       <c r="AO31" s="1"/>
@@ -2906,17 +2997,19 @@
       <c r="D32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F32" s="1">
-        <f t="shared" si="0"/>
-        <v>1.67</v>
+        <f t="shared" si="2"/>
+        <v>3.33</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="1"/>
-        <v>1.67</v>
+        <f t="shared" si="0"/>
+        <v>3.33</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I32" s="2"/>
@@ -2933,14 +3026,14 @@
         <v>80</v>
       </c>
       <c r="AJ32" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AK32" s="1">
         <v>10</v>
       </c>
       <c r="AL32" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AM32" s="1"/>
       <c r="AN32" s="1"/>
@@ -2968,15 +3061,15 @@
         <v>48</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I33" s="2"/>
@@ -3024,17 +3117,19 @@
       <c r="D34" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F34" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="1"/>
-        <v>3.33</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I34" s="2"/>
@@ -3050,7 +3145,7 @@
       <c r="AI34" s="1"/>
       <c r="AJ34" s="1">
         <f>SUM(AJ26:AJ33)</f>
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="AK34" s="1">
         <f>SUM(AK26:AK33)</f>
@@ -3058,7 +3153,7 @@
       </c>
       <c r="AL34" s="3">
         <f t="shared" si="4"/>
-        <v>0.91666666666666663</v>
+        <v>0.85</v>
       </c>
       <c r="AM34" s="1"/>
       <c r="AN34" s="1"/>
@@ -3082,17 +3177,19 @@
       <c r="D35" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F35" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" si="1"/>
-        <v>4.33</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I35" s="2" t="s">
@@ -3135,17 +3232,19 @@
       <c r="D36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.67</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I36" s="2"/>
@@ -3192,17 +3291,19 @@
       <c r="D37" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.33</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.33</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I37" s="2"/>
@@ -3219,14 +3320,14 @@
         <v>87</v>
       </c>
       <c r="AJ37" s="1">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="AK37" s="1">
         <v>80</v>
       </c>
       <c r="AL37" s="3">
         <f>AJ37/AK37</f>
-        <v>0.27500000000000002</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="AM37" s="1"/>
       <c r="AN37" s="1"/>
@@ -3254,15 +3355,15 @@
         <v>49</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.67</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I38" s="2"/>
@@ -3278,15 +3379,15 @@
       <c r="AI38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AJ38" s="5">
-        <v>100</v>
+      <c r="AJ38" s="1">
+        <v>50</v>
       </c>
       <c r="AK38" s="1">
         <v>100</v>
       </c>
       <c r="AL38" s="3">
         <f>AJ38/AK38</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AM38" s="1"/>
       <c r="AN38" s="1"/>
@@ -3310,17 +3411,19 @@
       <c r="D39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F39" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="H39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="I39" s="2" t="s">
@@ -3336,7 +3439,6 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="4"/>
       <c r="AI39" s="1"/>
-      <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
       <c r="AL39" s="1"/>
       <c r="AM39" s="1"/>
@@ -3361,17 +3463,19 @@
       <c r="D40" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F40" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G40" s="2">
-        <f t="shared" si="1"/>
-        <v>4.33</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I40" s="2" t="s">
@@ -3402,17 +3506,19 @@
       <c r="D41" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E41" s="2"/>
+      <c r="E41" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F41" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.67</v>
       </c>
       <c r="G41" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.67</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I41" s="2"/>
@@ -3439,17 +3545,19 @@
       <c r="D42" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="F42" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G42" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I42" s="2"/>
@@ -3476,18 +3584,20 @@
       <c r="D43" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E43" s="2"/>
+      <c r="E43" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F43" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G43" s="2">
-        <f t="shared" si="1"/>
-        <v>4.83</v>
+        <f t="shared" si="0"/>
+        <v>7.5</v>
       </c>
       <c r="H43" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+        <f t="shared" si="1"/>
+        <v>2.5</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2" t="s">
@@ -3501,8 +3611,12 @@
       <c r="N43" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
+      <c r="O43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q43" s="2"/>
       <c r="R43" s="4"/>
     </row>
@@ -3519,18 +3633,20 @@
       <c r="D44" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E44" s="2"/>
+      <c r="E44" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F44" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G44" s="2">
-        <f t="shared" si="1"/>
-        <v>4.83</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2" t="s">
@@ -3544,7 +3660,9 @@
         <v>48</v>
       </c>
       <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
+      <c r="O44" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="4"/>
@@ -3562,18 +3680,20 @@
       <c r="D45" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E45" s="2"/>
+      <c r="E45" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F45" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G45" s="2">
-        <f t="shared" si="1"/>
-        <v>5.83</v>
+        <f t="shared" si="0"/>
+        <v>8.5</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" si="2"/>
-        <v>2.5</v>
+        <f t="shared" si="1"/>
+        <v>3.5</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>48</v>
@@ -3591,8 +3711,12 @@
       <c r="N45" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
+      <c r="O45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="4"/>
     </row>
@@ -3609,17 +3733,19 @@
       <c r="D46" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F46" s="1">
-        <f t="shared" si="0"/>
-        <v>3.33</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="G46" s="2">
-        <f t="shared" si="1"/>
-        <v>3.33</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="H46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I46" s="2"/>
@@ -3649,7 +3775,7 @@
       </c>
       <c r="E47" s="1">
         <f>COUNTA(E2:E46)</f>
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="2"/>
@@ -3675,15 +3801,15 @@
       </c>
       <c r="N47" s="1">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O47" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P47" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="Q47" s="1">
         <f t="shared" si="5"/>
@@ -3707,7 +3833,7 @@
       </c>
       <c r="E48" s="3">
         <f>E47/$A$47</f>
-        <v>0.24444444444444444</v>
+        <v>1</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="2"/>
@@ -3736,15 +3862,15 @@
       </c>
       <c r="N48" s="3">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="O48" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="P48" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="Q48" s="3">
         <f t="shared" si="6"/>

</xml_diff>